<commit_message>
Ajout Fichier VS pour Prototype App Local
</commit_message>
<xml_diff>
--- a/Dictionnaire des données.xlsx
+++ b/Dictionnaire des données.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="405" windowWidth="19200" windowHeight="7410" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="405" windowWidth="19200" windowHeight="7410" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Feuil4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="166">
   <si>
     <t>Contraintes</t>
   </si>
@@ -442,6 +443,78 @@
   </si>
   <si>
     <t>Spectacles de cette salle</t>
+  </si>
+  <si>
+    <t># Sprint</t>
+  </si>
+  <si>
+    <t>Étapes à faire dans le sprint</t>
+  </si>
+  <si>
+    <t>Effort en heure</t>
+  </si>
+  <si>
+    <t>Sprint 1 (24 avril au 1 mai)</t>
+  </si>
+  <si>
+    <t>Sprint 0 (17 avril au 24 avril)</t>
+  </si>
+  <si>
+    <t>Sprint 2 (1 mai au 8 mai)</t>
+  </si>
+  <si>
+    <t>Sprint 3 (8 mai au 15 mai)</t>
+  </si>
+  <si>
+    <t>Sprint 4 (15 mai au 19 mai)</t>
+  </si>
+  <si>
+    <t>Analyse du projet                             Modélisation de la BD                   Modèle Relationnel      Prototype Application Locale</t>
+  </si>
+  <si>
+    <t>Interface Application Web   Implémentation des différentes fonctionnalités de recherche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implémentation de la BD             Création des packages/triggers                         </t>
+  </si>
+  <si>
+    <t>Implémentation du panier et du système de facture Implémentation des comptes utilisateurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application Locale               Debug App Web et Locale </t>
+  </si>
+  <si>
+    <t>Choses à faire</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Temps</t>
+  </si>
+  <si>
+    <t>Mélissa</t>
+  </si>
+  <si>
+    <t>Frederic</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Insertion de base</t>
+  </si>
+  <si>
+    <t>Charlie, Melissa et Frederic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package Recherche                - Fonctions et Procédures </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package Panier/Facture                - Fonctions et Procédures </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package App locale                - Fonctions et Procédures </t>
   </si>
 </sst>
 </file>
@@ -730,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -860,6 +933,47 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1129,7 +1243,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1905,8 +2019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F9:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:H30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2173,4 +2287,150 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="62">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="62">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="61" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="64" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="65">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="66" t="s">
+        <v>163</v>
+      </c>
+      <c r="G19" s="58" t="s">
+        <v>159</v>
+      </c>
+      <c r="H19" s="60">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F20" s="67" t="s">
+        <v>164</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="H20" s="62">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F21" s="67" t="s">
+        <v>165</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="H21" s="62">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="68" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="H22" s="65">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>